<commit_message>
fix ram, fix Obctlr
</commit_message>
<xml_diff>
--- a/RTLConnection_axis.xlsx
+++ b/RTLConnection_axis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\MyData\Git\Proj\EP_pcie\my_design\pcie_ep_dma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B36DEA-050A-4795-ACBC-F5878D06D93F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEF6CA1-3740-4E4C-A432-F8101EAB78A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1209" yWindow="-103" windowWidth="20837" windowHeight="12549" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1209" yWindow="-103" windowWidth="20837" windowHeight="12549" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,14 @@
     <sheet name="ObCtlr" sheetId="4" r:id="rId4"/>
     <sheet name="Mem" sheetId="5" r:id="rId5"/>
     <sheet name="Crypto" sheetId="6" r:id="rId6"/>
-    <sheet name="jtag" sheetId="7" r:id="rId7"/>
+    <sheet name="jtag_axi" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="185">
   <si>
     <t>Port Direction</t>
   </si>
@@ -569,6 +569,18 @@
   </si>
   <si>
     <t>ObRamValid</t>
+  </si>
+  <si>
+    <t>JtagAxi</t>
+  </si>
+  <si>
+    <t>jtag_axi</t>
+  </si>
+  <si>
+    <t>JtagEn</t>
+  </si>
+  <si>
+    <t>&lt;Jtag&gt;~</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR35" sqref="AR35"/>
+    <sheetView topLeftCell="AF24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO35" sqref="AO35:AS44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1224,7 +1236,7 @@
         <v>109</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="AS1" s="5" t="s">
         <v>121</v>
@@ -1634,9 +1646,6 @@
       </c>
       <c r="AE10" s="14"/>
       <c r="AJ10" s="14"/>
-      <c r="AQ10" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="AT10" s="24"/>
       <c r="AU10" s="25"/>
       <c r="AV10" s="25"/>
@@ -1737,15 +1746,6 @@
         <v>6</v>
       </c>
       <c r="AJ12" s="14"/>
-      <c r="AO12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ12" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR12" s="13" t="s">
-        <v>131</v>
-      </c>
       <c r="AT12" s="24"/>
       <c r="AU12" s="25"/>
       <c r="AV12" s="25"/>
@@ -1808,15 +1808,6 @@
       <c r="AL13" s="1"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="2"/>
-      <c r="AO13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ13" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AR13" s="13" t="s">
-        <v>132</v>
-      </c>
       <c r="AT13" s="24"/>
       <c r="AU13" s="25"/>
       <c r="AV13" s="25"/>
@@ -1872,15 +1863,6 @@
       <c r="AN14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AO14" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ14" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="AR14" s="13" t="s">
-        <v>133</v>
-      </c>
       <c r="AT14" s="24"/>
       <c r="AU14" s="25"/>
       <c r="AV14" s="25"/>
@@ -1936,15 +1918,6 @@
       <c r="AN15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AO15" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ15" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AR15" s="13" t="s">
-        <v>134</v>
-      </c>
       <c r="AT15" s="24"/>
       <c r="AU15" s="25"/>
       <c r="AV15" s="25"/>
@@ -1983,15 +1956,6 @@
       <c r="AN16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AO16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ16" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR16" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="AT16" s="24"/>
       <c r="AU16" s="25"/>
       <c r="AV16" s="25"/>
@@ -2016,15 +1980,6 @@
       </c>
       <c r="AD17" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="AO17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ17" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AR17" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="AT17" s="24"/>
       <c r="AU17" s="25"/>
@@ -2057,15 +2012,6 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="14"/>
-      <c r="AO18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ18" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="AR18" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="AT18" s="24"/>
       <c r="AU18" s="25"/>
       <c r="AV18" s="25"/>
@@ -2102,15 +2048,6 @@
         <v>6</v>
       </c>
       <c r="AJ19" s="14"/>
-      <c r="AO19" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ19" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AR19" s="13" t="s">
-        <v>138</v>
-      </c>
       <c r="AT19" s="24"/>
       <c r="AU19" s="25"/>
       <c r="AV19" s="25"/>
@@ -2356,12 +2293,6 @@
       <c r="AN24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AP24" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AQ24" s="1"/>
-      <c r="AR24" s="1"/>
-      <c r="AS24" s="2"/>
       <c r="AT24" s="24"/>
       <c r="AU24" s="25"/>
       <c r="AV24" s="25"/>
@@ -2391,12 +2322,6 @@
       <c r="AD25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AF25" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="2:50" x14ac:dyDescent="0.4">
       <c r="K26" s="14"/>
@@ -2427,60 +2352,12 @@
       <c r="AD26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE26" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG26" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH26" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="AI26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO26" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ26" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR26" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="AS26" s="7" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="27" spans="2:50" x14ac:dyDescent="0.4">
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="N27" s="14"/>
       <c r="T27" s="8"/>
-      <c r="AE27" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG27" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH27" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AI27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO27" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ27" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR27" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS27" s="7" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="28" spans="2:50" x14ac:dyDescent="0.4">
       <c r="Q28" s="11" t="s">
@@ -2495,18 +2372,6 @@
       <c r="W28" s="11"/>
       <c r="X28" s="11"/>
       <c r="Y28" s="6"/>
-      <c r="AE28" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG28" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH28" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="AI28" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ28" s="13" t="s">
         <v>31</v>
       </c>
@@ -2518,18 +2383,6 @@
       </c>
       <c r="AN28" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="AO28" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ28" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR28" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="AS28" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="29" spans="2:50" x14ac:dyDescent="0.4">
@@ -2561,18 +2414,6 @@
       <c r="Y29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE29" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG29" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH29" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AI29" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ29" s="13" t="s">
         <v>29</v>
       </c>
@@ -2584,18 +2425,6 @@
       </c>
       <c r="AN29" s="13" t="s">
         <v>178</v>
-      </c>
-      <c r="AO29" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ29" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR29" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AS29" s="7" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="30" spans="2:50" x14ac:dyDescent="0.4">
@@ -2622,30 +2451,6 @@
       <c r="Y30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE30" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG30" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH30" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AI30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO30" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ30" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR30" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AS30" s="7" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="31" spans="2:50" x14ac:dyDescent="0.4">
       <c r="I31" s="14"/>
@@ -2677,18 +2482,6 @@
       <c r="Y31" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE31" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG31" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="AH31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI31" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ31" s="14" t="s">
         <v>31</v>
       </c>
@@ -2700,18 +2493,6 @@
       </c>
       <c r="AN31" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="AO31" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ31" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="AR31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="AS31" s="7" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="32" spans="2:50" x14ac:dyDescent="0.4">
@@ -2743,18 +2524,6 @@
       <c r="Y32" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG32" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH32" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI32" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="AJ32" s="14" t="s">
         <v>29</v>
       </c>
@@ -2766,18 +2535,6 @@
       </c>
       <c r="AN32" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="AO32" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ32" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR32" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="AS32" s="7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.4">
@@ -2842,36 +2599,12 @@
       <c r="Y34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE34" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI34" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="AK34" s="17" t="s">
         <v>52</v>
       </c>
       <c r="AL34" s="17"/>
       <c r="AM34" s="17"/>
       <c r="AN34" s="18"/>
-      <c r="AO34" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="AS34" s="7" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A35" s="14"/>
@@ -2900,30 +2633,18 @@
       <c r="Y35" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE35" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG35" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH35" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="AI35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO35" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ35" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR35" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="AS35" s="7" t="s">
-        <v>147</v>
-      </c>
+      <c r="AF35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="2"/>
+      <c r="AP35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AQ35" s="1"/>
+      <c r="AR35" s="1"/>
+      <c r="AS35" s="2"/>
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A36" s="14"/>
@@ -2953,23 +2674,17 @@
       <c r="AE36" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AG36" s="13" t="s">
-        <v>127</v>
-      </c>
       <c r="AH36" s="13" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="AI36" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO36" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ36" s="13" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="AR36" s="13" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="AS36" s="7" t="s">
         <v>6</v>
@@ -2982,30 +2697,6 @@
       <c r="E37" s="10"/>
       <c r="I37" s="14"/>
       <c r="T37" s="8"/>
-      <c r="AE37" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG37" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH37" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="AI37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO37" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ37" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR37" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS37" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.4">
       <c r="A38" s="14"/>
@@ -3026,25 +2717,25 @@
       <c r="AC38" s="11"/>
       <c r="AD38" s="6"/>
       <c r="AE38" s="13" t="s">
-        <v>169</v>
+        <v>31</v>
       </c>
       <c r="AG38" s="13" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="AH38" s="13" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="AI38" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO38" s="13" t="s">
-        <v>168</v>
+        <v>31</v>
       </c>
       <c r="AQ38" s="13" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="AR38" s="13" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="AS38" s="7" t="s">
         <v>6</v>
@@ -3082,25 +2773,25 @@
         <v>6</v>
       </c>
       <c r="AE39" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AG39" s="13" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="AH39" s="13" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="AI39" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO39" s="13" t="s">
         <v>29</v>
       </c>
       <c r="AQ39" s="13" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="AR39" s="13" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="AS39" s="7" t="s">
         <v>6</v>
@@ -3130,23 +2821,17 @@
       <c r="AE40" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AG40" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="AH40" s="13" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="AI40" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO40" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ40" s="13" t="s">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="AR40" s="13" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="AS40" s="7" t="s">
         <v>6</v>
@@ -3196,25 +2881,25 @@
         <v>6</v>
       </c>
       <c r="AE42" s="13" t="s">
-        <v>169</v>
+        <v>31</v>
       </c>
       <c r="AG42" s="13" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="AH42" s="13" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="AI42" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO42" s="13" t="s">
-        <v>168</v>
+        <v>31</v>
       </c>
       <c r="AQ42" s="13" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="AR42" s="13" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="AS42" s="7" t="s">
         <v>6</v>
@@ -3251,22 +2936,22 @@
         <v>31</v>
       </c>
       <c r="AG43" s="13" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="AH43" s="13" t="s">
-        <v>154</v>
+        <v>55</v>
       </c>
       <c r="AI43" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO43" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AQ43" s="13" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="AR43" s="13" t="s">
-        <v>154</v>
+        <v>55</v>
       </c>
       <c r="AS43" s="7" t="s">
         <v>6</v>
@@ -3276,25 +2961,19 @@
       <c r="I44" s="14"/>
       <c r="T44" s="8"/>
       <c r="AE44" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG44" s="13" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="AH44" s="13" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="AI44" s="7" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="AO44" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ44" s="13" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="AR44" s="13" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="AS44" s="7" t="s">
         <v>6</v>
@@ -3314,30 +2993,6 @@
       <c r="W45" s="11"/>
       <c r="X45" s="11"/>
       <c r="Y45" s="6"/>
-      <c r="AE45" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG45" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH45" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="AI45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO45" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ45" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR45" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="AS45" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.4">
       <c r="I46" s="14"/>
@@ -3366,30 +3021,6 @@
       <c r="Y46" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE46" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG46" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH46" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="AI46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO46" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ46" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR46" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="AS46" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.4">
       <c r="P47" s="14" t="s">
@@ -3411,30 +3042,6 @@
       <c r="Y47" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE47" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG47" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH47" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="AI47" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO47" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ47" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR47" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="AS47" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.4">
       <c r="P48" s="14" t="s">
@@ -3456,30 +3063,6 @@
       <c r="Y48" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG48" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH48" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="AI48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO48" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ48" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR48" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="AS48" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="49" spans="16:50" x14ac:dyDescent="0.4">
       <c r="P49" s="14" t="s">
@@ -3501,30 +3084,6 @@
       <c r="Y49" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AE49" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG49" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH49" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AI49" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO49" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ49" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR49" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="AS49" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="50" spans="16:50" x14ac:dyDescent="0.4">
       <c r="P50" s="14" t="s">
@@ -3550,30 +3109,6 @@
         <v>95</v>
       </c>
       <c r="Y50" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE50" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG50" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH50" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="AI50" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO50" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ50" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR50" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="AS50" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3599,165 +3134,21 @@
       <c r="AB52" s="17"/>
       <c r="AC52" s="17"/>
       <c r="AD52" s="18"/>
-      <c r="AE52" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG52" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH52" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="AI52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO52" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ52" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR52" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="AS52" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="53" spans="16:50" x14ac:dyDescent="0.4">
       <c r="T53" s="8"/>
-      <c r="AE53" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG53" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH53" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="AI53" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO53" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ53" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR53" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="AS53" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="54" spans="16:50" x14ac:dyDescent="0.4">
       <c r="T54" s="8"/>
-      <c r="AE54" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG54" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH54" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="AI54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO54" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ54" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR54" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="AS54" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="55" spans="16:50" x14ac:dyDescent="0.4">
       <c r="T55" s="8"/>
-      <c r="AE55" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG55" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH55" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="AI55" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO55" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ55" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR55" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="AS55" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="56" spans="16:50" x14ac:dyDescent="0.4">
       <c r="T56" s="8"/>
-      <c r="AE56" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG56" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH56" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="AI56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO56" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ56" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR56" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="AS56" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="57" spans="16:50" x14ac:dyDescent="0.4">
       <c r="T57" s="8"/>
-      <c r="AE57" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG57" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH57" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="AI57" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AO57" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ57" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AR57" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="AS57" s="7" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="58" spans="16:50" x14ac:dyDescent="0.4">
       <c r="T58" s="8"/>
@@ -6053,10 +5444,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA65B74B-5DA1-4137-A045-0809C3DDDFED}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6065,9 +5456,10 @@
     <col min="2" max="2" width="4.61328125" customWidth="1"/>
     <col min="3" max="3" width="6.61328125" customWidth="1"/>
     <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -6077,8 +5469,17 @@
       <c r="E1" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="13"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
@@ -6086,15 +5487,27 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F2" s="13"/>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>28</v>
@@ -6102,8 +5515,15 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
         <v>168</v>
       </c>
@@ -6113,10 +5533,21 @@
         <v>129</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
@@ -6126,687 +5557,982 @@
         <v>130</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="13"/>
+      <c r="B8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
-        <v>123</v>
-      </c>
+      <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="I12" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="I13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" s="13"/>
       <c r="B14" s="13"/>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="I14" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="I15" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="13" t="s">
-        <v>124</v>
-      </c>
+      <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" s="13"/>
       <c r="B18" s="13"/>
-      <c r="C18" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="13"/>
+      <c r="B19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F20" s="13"/>
+      <c r="G20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="13"/>
-      <c r="B24" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F24" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="F25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="13"/>
       <c r="B26" s="13"/>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A27" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13" t="s">
+      <c r="I30" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A28" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13" t="s">
+      <c r="I31" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A29" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A30" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A31" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A32" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="I32" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="F33" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A35" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A35" s="13"/>
       <c r="B35" s="13"/>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="7"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A36" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A37" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A38" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A39" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A40" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="I40" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
       <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A42" s="13" t="s">
+      <c r="F41" s="13" t="s">
         <v>168</v>
       </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A42" s="13"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A43" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13" t="s">
+      <c r="I49" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A44" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A45" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A46" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A47" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A48" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A49" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A50" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="I50" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A52" s="13" t="s">
+      <c r="F51" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A53" s="13" t="s">
+      <c r="G52" s="13"/>
+      <c r="H52" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A54" s="13" t="s">
-        <v>168</v>
-      </c>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A54" s="13"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A55" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="7"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A55" s="13"/>
       <c r="B55" s="13"/>
-      <c r="C55" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A56" s="13" t="s">
-        <v>168</v>
-      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A56" s="13"/>
       <c r="B56" s="13"/>
-      <c r="C56" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A57" s="13" t="s">
-        <v>168</v>
-      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="18"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A57" s="13"/>
       <c r="B57" s="13"/>
-      <c r="C57" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60" s="13"/>
-      <c r="B60" s="17" t="s">
-        <v>52</v>
-      </c>
+      <c r="B60" s="17"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17"/>
       <c r="E60" s="18"/>

</xml_diff>

<commit_message>
update excel connection file
</commit_message>
<xml_diff>
--- a/RTLConnection_axis.xlsx
+++ b/RTLConnection_axis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\MyData\Git\Proj\EP_pcie\my_design\pcie_ep_dma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Crypto\vivado\PCIE_TOP\pcie_dma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEF6CA1-3740-4E4C-A432-F8101EAB78A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1209" yWindow="-103" windowWidth="20837" windowHeight="12549" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="-105" windowWidth="20835" windowHeight="12555" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="185">
   <si>
     <t>Port Direction</t>
   </si>
@@ -535,9 +534,6 @@
     <t xml:space="preserve">I </t>
   </si>
   <si>
-    <t xml:space="preserve">O </t>
-  </si>
-  <si>
     <t>AXI</t>
   </si>
   <si>
@@ -581,12 +577,15 @@
   </si>
   <si>
     <t>&lt;Jtag&gt;~</t>
+  </si>
+  <si>
+    <t>JTAG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1026,19 +1025,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1055,12 +1054,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1076,12 +1075,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1089,12 +1088,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1110,12 +1109,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1129,61 +1128,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX197"/>
   <sheetViews>
-    <sheetView topLeftCell="AF24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO35" sqref="AO35:AS44"/>
+    <sheetView topLeftCell="Z28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM52" sqref="AM52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.15234375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.3828125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="18.23046875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="11.765625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.23046875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="2.15234375" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.15234375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="9.23046875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.07421875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="9.23046875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="3.4609375" style="13" customWidth="1"/>
-    <col min="12" max="12" width="3.921875" style="13" customWidth="1"/>
-    <col min="13" max="13" width="3.61328125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="4.4609375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="11.3828125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="2.15234375" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.15234375" style="14" customWidth="1"/>
-    <col min="18" max="18" width="17.07421875" style="13" customWidth="1"/>
-    <col min="19" max="19" width="22.07421875" style="13" customWidth="1"/>
-    <col min="20" max="20" width="8.84375" style="7" customWidth="1"/>
-    <col min="21" max="21" width="2.15234375" style="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.23046875" style="13" customWidth="1"/>
-    <col min="24" max="24" width="22.69140625" style="13" customWidth="1"/>
-    <col min="25" max="25" width="9.921875" style="7" customWidth="1"/>
-    <col min="26" max="26" width="2.15234375" style="14" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="9.23046875" style="13" customWidth="1"/>
-    <col min="29" max="29" width="19.15234375" style="13" customWidth="1"/>
-    <col min="30" max="30" width="6.84375" style="7" customWidth="1"/>
-    <col min="31" max="31" width="2.15234375" style="13" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.23046875" style="13" customWidth="1"/>
-    <col min="34" max="34" width="12.921875" style="13" customWidth="1"/>
-    <col min="35" max="35" width="9.23046875" style="7" customWidth="1"/>
-    <col min="36" max="36" width="2.15234375" style="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="9.23046875" style="13" customWidth="1"/>
-    <col min="40" max="40" width="9.23046875" style="7" customWidth="1"/>
-    <col min="41" max="41" width="2.15234375" style="13" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="9.23046875" style="13" customWidth="1"/>
-    <col min="44" max="44" width="16.3828125" style="13" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.23046875" style="7"/>
-    <col min="46" max="46" width="4.69140625" style="13" customWidth="1"/>
-    <col min="47" max="49" width="9.23046875" style="13"/>
-    <col min="50" max="50" width="9.23046875" style="7"/>
-    <col min="51" max="16384" width="9.23046875" style="13"/>
+    <col min="1" max="1" width="2.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="3.85546875" style="13" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" style="13" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" style="13" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.140625" style="14" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" style="13" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.28515625" style="13" customWidth="1"/>
+    <col min="24" max="24" width="22.7109375" style="13" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" style="7" customWidth="1"/>
+    <col min="26" max="26" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="9.28515625" style="13" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" style="13" customWidth="1"/>
+    <col min="30" max="30" width="6.85546875" style="7" customWidth="1"/>
+    <col min="31" max="31" width="2.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.28515625" style="13" customWidth="1"/>
+    <col min="34" max="34" width="12.85546875" style="13" customWidth="1"/>
+    <col min="35" max="35" width="9.28515625" style="7" customWidth="1"/>
+    <col min="36" max="36" width="2.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="9.28515625" style="13" customWidth="1"/>
+    <col min="40" max="40" width="9.28515625" style="7" customWidth="1"/>
+    <col min="41" max="41" width="2.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="9.28515625" style="13" customWidth="1"/>
+    <col min="44" max="44" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.28515625" style="7"/>
+    <col min="46" max="46" width="4.7109375" style="13" customWidth="1"/>
+    <col min="47" max="49" width="9.28515625" style="13"/>
+    <col min="50" max="50" width="9.28515625" style="7"/>
+    <col min="51" max="16384" width="9.28515625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:50" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D1" s="12" t="s">
         <v>18</v>
       </c>
@@ -1236,14 +1235,14 @@
         <v>109</v>
       </c>
       <c r="AR1" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AS1" s="5" t="s">
         <v>121</v>
       </c>
       <c r="AX1" s="5"/>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
@@ -1298,11 +1297,11 @@
       <c r="AR2" s="1"/>
       <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:50" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:50" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="Q4" s="3" t="s">
@@ -1348,7 +1347,7 @@
       <c r="AW4" s="25"/>
       <c r="AX4" s="8"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="F5" s="14" t="s">
@@ -1420,7 +1419,7 @@
       <c r="AW5" s="25"/>
       <c r="AX5" s="8"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="F6" s="14" t="s">
@@ -1499,7 +1498,7 @@
       <c r="AW6" s="25"/>
       <c r="AX6" s="8"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="F7" s="14" t="s">
@@ -1526,7 +1525,7 @@
       <c r="AW7" s="25"/>
       <c r="AX7" s="8"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>31</v>
       </c>
@@ -1569,7 +1568,7 @@
       <c r="AW8" s="25"/>
       <c r="AX8" s="8"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
@@ -1612,7 +1611,7 @@
       <c r="AW9" s="25"/>
       <c r="AX9" s="8"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>31</v>
       </c>
@@ -1652,7 +1651,7 @@
       <c r="AW10" s="25"/>
       <c r="AX10" s="8"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="G11" s="17" t="s">
         <v>52</v>
       </c>
@@ -1696,7 +1695,7 @@
       <c r="AW11" s="25"/>
       <c r="AX11" s="8"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
@@ -1752,7 +1751,7 @@
       <c r="AW12" s="25"/>
       <c r="AX12" s="8"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
@@ -1814,7 +1813,7 @@
       <c r="AW13" s="25"/>
       <c r="AX13" s="8"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>29</v>
       </c>
       <c r="AG14" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AH14" s="13" t="s">
         <v>102</v>
@@ -1855,7 +1854,7 @@
         <v>31</v>
       </c>
       <c r="AL14" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AM14" s="13" t="s">
         <v>56</v>
@@ -1869,7 +1868,7 @@
       <c r="AW14" s="25"/>
       <c r="AX14" s="8"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>31</v>
       </c>
@@ -1924,7 +1923,7 @@
       <c r="AW15" s="25"/>
       <c r="AX15" s="8"/>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="T16" s="8"/>
       <c r="AA16" s="3" t="s">
         <v>44</v>
@@ -1936,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="AG16" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AH16" s="13" t="s">
         <v>104</v>
@@ -1948,7 +1947,7 @@
         <v>29</v>
       </c>
       <c r="AL16" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AM16" s="13" t="s">
         <v>63</v>
@@ -1962,7 +1961,7 @@
       <c r="AW16" s="25"/>
       <c r="AX16" s="8"/>
     </row>
-    <row r="17" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>52</v>
       </c>
@@ -1987,7 +1986,7 @@
       <c r="AW17" s="25"/>
       <c r="AX17" s="8"/>
     </row>
-    <row r="18" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -2018,7 +2017,7 @@
       <c r="AW18" s="25"/>
       <c r="AX18" s="8"/>
     </row>
-    <row r="19" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -2054,7 +2053,7 @@
       <c r="AW19" s="25"/>
       <c r="AX19" s="8"/>
     </row>
-    <row r="20" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="Q20" s="3" t="s">
@@ -2088,7 +2087,7 @@
       <c r="AW20" s="25"/>
       <c r="AX20" s="8"/>
     </row>
-    <row r="21" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="N21" s="14"/>
@@ -2138,7 +2137,7 @@
       <c r="AW21" s="25"/>
       <c r="AX21" s="8"/>
     </row>
-    <row r="22" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="N22" s="14"/>
@@ -2155,7 +2154,7 @@
         <v>31</v>
       </c>
       <c r="AG22" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AH22" s="13" t="s">
         <v>105</v>
@@ -2167,7 +2166,7 @@
         <v>29</v>
       </c>
       <c r="AL22" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AM22" s="13" t="s">
         <v>55</v>
@@ -2181,7 +2180,7 @@
       <c r="AW22" s="25"/>
       <c r="AX22" s="8"/>
     </row>
-    <row r="23" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="N23" s="14"/>
@@ -2240,7 +2239,7 @@
       <c r="AW23" s="25"/>
       <c r="AX23" s="8"/>
     </row>
-    <row r="24" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="N24" s="14"/>
@@ -2273,7 +2272,7 @@
         <v>31</v>
       </c>
       <c r="AG24" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AH24" s="13" t="s">
         <v>107</v>
@@ -2285,7 +2284,7 @@
         <v>29</v>
       </c>
       <c r="AL24" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AM24" s="13" t="s">
         <v>62</v>
@@ -2299,7 +2298,7 @@
       <c r="AW24" s="25"/>
       <c r="AX24" s="8"/>
     </row>
-    <row r="25" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
       <c r="N25" s="14"/>
@@ -2323,7 +2322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
       <c r="N26" s="14"/>
@@ -2353,13 +2352,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="N27" s="14"/>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:50" x14ac:dyDescent="0.25">
       <c r="Q28" s="11" t="s">
         <v>72</v>
       </c>
@@ -2379,13 +2378,13 @@
         <v>47</v>
       </c>
       <c r="AM28" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AN28" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="2:50" x14ac:dyDescent="0.4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="2:50" x14ac:dyDescent="0.25">
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
       <c r="M29" s="15"/>
@@ -2421,13 +2420,13 @@
         <v>47</v>
       </c>
       <c r="AM29" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AN29" s="13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="2:50" x14ac:dyDescent="0.4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="2:50" x14ac:dyDescent="0.25">
       <c r="I30" s="14"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
@@ -2452,7 +2451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:50" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:50" x14ac:dyDescent="0.25">
       <c r="I31" s="14"/>
       <c r="K31" s="14"/>
       <c r="L31" s="14"/>
@@ -2489,13 +2488,13 @@
         <v>47</v>
       </c>
       <c r="AM31" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AN31" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="2:50" x14ac:dyDescent="0.4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="2:50" x14ac:dyDescent="0.25">
       <c r="I32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
@@ -2531,13 +2530,13 @@
         <v>47</v>
       </c>
       <c r="AM32" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AN32" s="13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="D33" s="14"/>
@@ -2565,7 +2564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="D34" s="14"/>
@@ -2606,7 +2605,7 @@
       <c r="AM34" s="17"/>
       <c r="AN34" s="18"/>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="D35" s="14"/>
@@ -2634,19 +2633,19 @@
         <v>6</v>
       </c>
       <c r="AF35" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
       <c r="AI35" s="2"/>
       <c r="AP35" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AQ35" s="1"/>
       <c r="AR35" s="1"/>
       <c r="AS35" s="2"/>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="D36" s="14"/>
@@ -2675,22 +2674,22 @@
         <v>31</v>
       </c>
       <c r="AH36" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI36" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="AI36" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="AO36" s="13" t="s">
         <v>31</v>
       </c>
       <c r="AR36" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AS36" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="D37" s="14"/>
@@ -2698,7 +2697,7 @@
       <c r="I37" s="14"/>
       <c r="T37" s="8"/>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="D38" s="14"/>
@@ -2726,7 +2725,7 @@
         <v>63</v>
       </c>
       <c r="AI38" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO38" s="13" t="s">
         <v>31</v>
@@ -2741,7 +2740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="D39" s="14"/>
@@ -2782,7 +2781,7 @@
         <v>56</v>
       </c>
       <c r="AI39" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO39" s="13" t="s">
         <v>29</v>
@@ -2797,7 +2796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I40" s="14"/>
       <c r="P40" s="14" t="s">
         <v>31</v>
@@ -2825,7 +2824,7 @@
         <v>60</v>
       </c>
       <c r="AI40" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO40" s="13" t="s">
         <v>31</v>
@@ -2837,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I41" s="14"/>
       <c r="P41" s="14" t="s">
         <v>31</v>
@@ -2859,7 +2858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I42" s="14"/>
       <c r="P42" s="14" t="s">
         <v>29</v>
@@ -2890,7 +2889,7 @@
         <v>62</v>
       </c>
       <c r="AI42" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO42" s="13" t="s">
         <v>31</v>
@@ -2905,7 +2904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I43" s="14"/>
       <c r="P43" s="14" t="s">
         <v>31</v>
@@ -2942,7 +2941,7 @@
         <v>55</v>
       </c>
       <c r="AI43" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO43" s="13" t="s">
         <v>31</v>
@@ -2957,7 +2956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I44" s="14"/>
       <c r="T44" s="8"/>
       <c r="AE44" s="13" t="s">
@@ -2967,7 +2966,7 @@
         <v>59</v>
       </c>
       <c r="AI44" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AO44" s="13" t="s">
         <v>31</v>
@@ -2979,7 +2978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I45" s="14"/>
       <c r="Q45" s="11" t="s">
         <v>90</v>
@@ -2994,7 +2993,7 @@
       <c r="X45" s="11"/>
       <c r="Y45" s="6"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="I46" s="14"/>
       <c r="P46" s="14" t="s">
         <v>29</v>
@@ -3022,7 +3021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="P47" s="14" t="s">
         <v>29</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="P48" s="14" t="s">
         <v>29</v>
       </c>
@@ -3064,7 +3063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="49" spans="16:50" x14ac:dyDescent="0.25">
       <c r="P49" s="14" t="s">
         <v>31</v>
       </c>
@@ -3085,7 +3084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="50" spans="16:50" x14ac:dyDescent="0.25">
       <c r="P50" s="14" t="s">
         <v>29</v>
       </c>
@@ -3112,10 +3111,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="51" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T51" s="8"/>
     </row>
-    <row r="52" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="52" spans="16:50" x14ac:dyDescent="0.25">
       <c r="Q52" s="17" t="s">
         <v>52</v>
       </c>
@@ -3135,28 +3134,28 @@
       <c r="AC52" s="17"/>
       <c r="AD52" s="18"/>
     </row>
-    <row r="53" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="53" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T53" s="8"/>
     </row>
-    <row r="54" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="54" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T54" s="8"/>
     </row>
-    <row r="55" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="55" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T55" s="8"/>
     </row>
-    <row r="56" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="56" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T56" s="8"/>
     </row>
-    <row r="57" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="57" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T57" s="8"/>
     </row>
-    <row r="58" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="58" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T58" s="8"/>
     </row>
-    <row r="59" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="59" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T59" s="8"/>
     </row>
-    <row r="60" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="60" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T60" s="8"/>
       <c r="AF60" s="17" t="s">
         <v>52</v>
@@ -3171,455 +3170,455 @@
       <c r="AR60" s="17"/>
       <c r="AS60" s="18"/>
     </row>
-    <row r="61" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="61" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T61" s="8"/>
     </row>
-    <row r="62" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="62" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T62" s="8"/>
       <c r="AU62" s="19"/>
       <c r="AV62" s="19"/>
       <c r="AW62" s="19"/>
       <c r="AX62" s="20"/>
     </row>
-    <row r="63" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="63" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T63" s="8"/>
       <c r="AU63" s="19"/>
       <c r="AV63" s="19"/>
       <c r="AW63" s="19"/>
       <c r="AX63" s="20"/>
     </row>
-    <row r="64" spans="16:50" x14ac:dyDescent="0.4">
+    <row r="64" spans="16:50" x14ac:dyDescent="0.25">
       <c r="T64" s="8"/>
       <c r="AU64" s="19"/>
       <c r="AV64" s="19"/>
       <c r="AW64" s="19"/>
       <c r="AX64" s="20"/>
     </row>
-    <row r="65" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="65" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T65" s="8"/>
       <c r="AU65" s="19"/>
       <c r="AV65" s="19"/>
       <c r="AW65" s="19"/>
       <c r="AX65" s="20"/>
     </row>
-    <row r="66" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="66" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T66" s="8"/>
       <c r="AU66" s="19"/>
       <c r="AV66" s="19"/>
       <c r="AW66" s="19"/>
       <c r="AX66" s="20"/>
     </row>
-    <row r="67" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="67" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T67" s="8"/>
       <c r="AU67" s="19"/>
       <c r="AV67" s="19"/>
       <c r="AW67" s="19"/>
       <c r="AX67" s="20"/>
     </row>
-    <row r="68" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="68" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T68" s="8"/>
       <c r="AU68" s="19"/>
       <c r="AV68" s="19"/>
       <c r="AW68" s="19"/>
       <c r="AX68" s="20"/>
     </row>
-    <row r="69" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="69" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T69" s="8"/>
       <c r="AU69" s="19"/>
       <c r="AV69" s="19"/>
       <c r="AW69" s="19"/>
       <c r="AX69" s="20"/>
     </row>
-    <row r="70" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="70" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T70" s="8"/>
       <c r="AU70" s="19"/>
       <c r="AV70" s="19"/>
       <c r="AW70" s="19"/>
       <c r="AX70" s="20"/>
     </row>
-    <row r="71" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="71" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T71" s="8"/>
       <c r="AU71" s="19"/>
       <c r="AV71" s="19"/>
       <c r="AW71" s="19"/>
       <c r="AX71" s="20"/>
     </row>
-    <row r="72" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="72" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T72" s="8"/>
     </row>
-    <row r="73" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="73" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T73" s="8"/>
     </row>
-    <row r="74" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="74" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T74" s="8"/>
     </row>
-    <row r="75" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="75" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T75" s="8"/>
     </row>
-    <row r="76" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="76" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T76" s="8"/>
     </row>
-    <row r="77" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="77" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T77" s="8"/>
     </row>
-    <row r="78" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="78" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T78" s="8"/>
     </row>
-    <row r="79" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="79" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T79" s="8"/>
     </row>
-    <row r="80" spans="20:50" x14ac:dyDescent="0.4">
+    <row r="80" spans="20:50" x14ac:dyDescent="0.25">
       <c r="T80" s="8"/>
     </row>
-    <row r="81" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="81" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T81" s="8"/>
     </row>
-    <row r="82" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="82" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T82" s="8"/>
     </row>
-    <row r="83" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="83" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T83" s="8"/>
     </row>
-    <row r="84" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="84" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T84" s="8"/>
     </row>
-    <row r="85" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="85" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T85" s="8"/>
     </row>
-    <row r="86" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="86" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T86" s="8"/>
     </row>
-    <row r="87" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="87" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T87" s="8"/>
     </row>
-    <row r="88" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="88" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T88" s="8"/>
     </row>
-    <row r="89" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="89" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T89" s="8"/>
     </row>
-    <row r="90" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="90" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T90" s="8"/>
     </row>
-    <row r="91" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="91" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T91" s="8"/>
     </row>
-    <row r="92" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="92" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T92" s="8"/>
     </row>
-    <row r="93" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="93" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T93" s="8"/>
     </row>
-    <row r="94" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="94" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T94" s="8"/>
     </row>
-    <row r="95" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="95" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T95" s="8"/>
     </row>
-    <row r="96" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="96" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T96" s="8"/>
     </row>
-    <row r="97" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="97" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T97" s="8"/>
     </row>
-    <row r="98" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="98" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T98" s="8"/>
     </row>
-    <row r="99" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="99" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T99" s="8"/>
     </row>
-    <row r="100" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="100" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T100" s="8"/>
     </row>
-    <row r="101" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="101" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T101" s="8"/>
     </row>
-    <row r="102" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="102" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T102" s="8"/>
     </row>
-    <row r="103" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="103" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T103" s="8"/>
     </row>
-    <row r="104" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="104" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T104" s="8"/>
     </row>
-    <row r="105" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="105" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T105" s="8"/>
     </row>
-    <row r="106" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="106" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T106" s="8"/>
     </row>
-    <row r="107" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="107" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T107" s="8"/>
     </row>
-    <row r="108" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="108" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T108" s="8"/>
     </row>
-    <row r="109" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="109" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T109" s="8"/>
     </row>
-    <row r="110" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="110" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T110" s="8"/>
     </row>
-    <row r="111" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="111" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T111" s="8"/>
     </row>
-    <row r="112" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="112" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T112" s="8"/>
     </row>
-    <row r="113" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="113" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T113" s="8"/>
     </row>
-    <row r="114" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="114" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T114" s="8"/>
     </row>
-    <row r="115" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="115" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T115" s="8"/>
     </row>
-    <row r="116" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="116" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T116" s="8"/>
     </row>
-    <row r="117" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="117" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T117" s="8"/>
     </row>
-    <row r="118" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="118" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T118" s="8"/>
     </row>
-    <row r="119" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="119" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T119" s="8"/>
     </row>
-    <row r="120" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="120" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T120" s="8"/>
     </row>
-    <row r="121" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="121" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T121" s="8"/>
     </row>
-    <row r="122" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="122" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T122" s="8"/>
     </row>
-    <row r="123" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="123" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T123" s="8"/>
     </row>
-    <row r="124" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="124" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T124" s="8"/>
     </row>
-    <row r="125" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="125" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T125" s="8"/>
     </row>
-    <row r="126" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="126" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T126" s="8"/>
     </row>
-    <row r="127" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="127" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T127" s="8"/>
     </row>
-    <row r="128" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="128" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T128" s="8"/>
     </row>
-    <row r="129" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="129" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T129" s="8"/>
     </row>
-    <row r="130" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="130" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T130" s="8"/>
     </row>
-    <row r="131" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="131" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T131" s="8"/>
     </row>
-    <row r="132" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="132" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T132" s="8"/>
     </row>
-    <row r="133" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="133" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T133" s="8"/>
     </row>
-    <row r="134" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="134" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T134" s="8"/>
     </row>
-    <row r="135" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="135" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T135" s="8"/>
     </row>
-    <row r="136" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="136" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T136" s="8"/>
     </row>
-    <row r="137" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="137" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T137" s="8"/>
     </row>
-    <row r="138" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="138" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T138" s="8"/>
     </row>
-    <row r="139" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="139" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T139" s="8"/>
     </row>
-    <row r="140" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="140" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T140" s="8"/>
     </row>
-    <row r="141" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="141" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T141" s="8"/>
     </row>
-    <row r="142" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="142" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T142" s="8"/>
     </row>
-    <row r="143" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="143" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T143" s="8"/>
     </row>
-    <row r="144" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="144" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T144" s="8"/>
     </row>
-    <row r="145" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="145" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T145" s="8"/>
     </row>
-    <row r="146" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="146" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T146" s="8"/>
     </row>
-    <row r="147" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="147" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T147" s="8"/>
     </row>
-    <row r="148" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="148" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T148" s="8"/>
     </row>
-    <row r="149" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="149" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T149" s="8"/>
     </row>
-    <row r="150" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="150" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T150" s="8"/>
     </row>
-    <row r="151" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="151" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T151" s="8"/>
     </row>
-    <row r="152" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="152" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T152" s="8"/>
     </row>
-    <row r="153" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="153" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T153" s="8"/>
     </row>
-    <row r="154" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="154" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T154" s="8"/>
     </row>
-    <row r="155" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="155" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T155" s="8"/>
     </row>
-    <row r="156" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="156" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T156" s="8"/>
     </row>
-    <row r="157" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="157" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T157" s="8"/>
     </row>
-    <row r="158" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="158" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T158" s="8"/>
     </row>
-    <row r="159" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="159" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T159" s="8"/>
     </row>
-    <row r="160" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="160" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T160" s="8"/>
     </row>
-    <row r="161" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="161" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T161" s="8"/>
     </row>
-    <row r="162" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="162" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T162" s="8"/>
     </row>
-    <row r="163" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="163" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T163" s="8"/>
     </row>
-    <row r="164" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="164" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T164" s="8"/>
     </row>
-    <row r="165" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="165" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T165" s="8"/>
     </row>
-    <row r="166" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="166" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T166" s="8"/>
     </row>
-    <row r="167" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="167" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T167" s="8"/>
     </row>
-    <row r="168" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="168" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T168" s="8"/>
     </row>
-    <row r="169" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="169" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T169" s="8"/>
     </row>
-    <row r="170" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="170" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T170" s="8"/>
     </row>
-    <row r="171" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="171" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T171" s="8"/>
     </row>
-    <row r="172" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="172" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T172" s="8"/>
     </row>
-    <row r="173" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="173" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T173" s="8"/>
     </row>
-    <row r="174" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="174" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T174" s="8"/>
     </row>
-    <row r="175" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="175" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T175" s="8"/>
     </row>
-    <row r="176" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="176" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T176" s="8"/>
     </row>
-    <row r="177" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="177" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T177" s="8"/>
     </row>
-    <row r="178" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="178" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T178" s="8"/>
     </row>
-    <row r="179" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="179" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T179" s="8"/>
     </row>
-    <row r="180" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="180" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T180" s="8"/>
     </row>
-    <row r="181" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="181" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T181" s="8"/>
     </row>
-    <row r="182" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="182" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T182" s="8"/>
     </row>
-    <row r="183" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="183" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T183" s="8"/>
     </row>
-    <row r="184" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="184" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T184" s="8"/>
     </row>
-    <row r="185" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="185" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T185" s="8"/>
     </row>
-    <row r="186" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="186" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T186" s="8"/>
     </row>
-    <row r="187" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="187" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T187" s="8"/>
     </row>
-    <row r="188" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="188" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T188" s="8"/>
     </row>
-    <row r="189" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="189" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T189" s="8"/>
     </row>
-    <row r="190" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="190" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T190" s="8"/>
     </row>
-    <row r="191" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="191" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T191" s="8"/>
     </row>
-    <row r="192" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="192" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T192" s="8"/>
     </row>
-    <row r="193" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="193" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T193" s="8"/>
     </row>
-    <row r="194" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="194" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T194" s="8"/>
     </row>
-    <row r="195" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="195" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T195" s="8"/>
     </row>
-    <row r="196" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="196" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T196" s="8"/>
     </row>
-    <row r="197" spans="20:20" x14ac:dyDescent="0.4">
+    <row r="197" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T197" s="8"/>
     </row>
   </sheetData>
@@ -3629,22 +3628,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:E52"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.15234375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23046875" style="13"/>
-    <col min="4" max="4" width="22.69140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.921875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="13"/>
+    <col min="4" max="4" width="22.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -3655,7 +3654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
@@ -3663,7 +3662,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -3671,7 +3670,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>31</v>
       </c>
@@ -3682,7 +3681,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -3693,7 +3692,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
@@ -3701,7 +3700,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -3715,7 +3714,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>31</v>
       </c>
@@ -3729,7 +3728,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
@@ -3743,7 +3742,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
@@ -3754,7 +3753,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>72</v>
       </c>
@@ -3776,7 +3775,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>29</v>
       </c>
@@ -3803,7 +3802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>29</v>
       </c>
@@ -3818,7 +3817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>29</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>29</v>
       </c>
@@ -3845,7 +3844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>31</v>
       </c>
@@ -3860,7 +3859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>31</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>29</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>90</v>
       </c>
@@ -3892,7 +3891,7 @@
       <c r="D45" s="11"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>31</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>31</v>
       </c>
@@ -3919,7 +3918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>31</v>
       </c>
@@ -3931,7 +3930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>29</v>
       </c>
@@ -3943,7 +3942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>31</v>
       </c>
@@ -3958,7 +3957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="17" t="s">
         <v>52</v>
       </c>
@@ -3972,22 +3971,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.15234375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23046875" style="13"/>
-    <col min="4" max="4" width="19.15234375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="13"/>
+    <col min="4" max="4" width="19.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -3998,7 +3997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
@@ -4006,7 +4005,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -4014,7 +4013,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>31</v>
       </c>
@@ -4025,7 +4024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -4036,7 +4035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>44</v>
       </c>
@@ -4044,7 +4043,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>31</v>
       </c>
@@ -4058,7 +4057,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>29</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>31</v>
       </c>
@@ -4086,7 +4085,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>29</v>
       </c>
@@ -4097,7 +4096,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>29</v>
       </c>
@@ -4111,7 +4110,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
@@ -4126,7 +4125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>31</v>
       </c>
@@ -4141,7 +4140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
@@ -4153,7 +4152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>31</v>
       </c>
@@ -4168,7 +4167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>83</v>
       </c>
@@ -4176,7 +4175,7 @@
       <c r="D38" s="11"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>29</v>
       </c>
@@ -4191,7 +4190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>29</v>
       </c>
@@ -4203,7 +4202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>29</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>31</v>
       </c>
@@ -4227,7 +4226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>29</v>
       </c>
@@ -4242,7 +4241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="17" t="s">
         <v>52</v>
       </c>
@@ -4256,30 +4255,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721A5B20-E329-4ED6-9EC7-6F1A7EBE8146}">
-  <dimension ref="A1:Y65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y68"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E58" sqref="A58:E58"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.15234375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23046875" style="13"/>
-    <col min="4" max="4" width="12.921875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.23046875" style="7"/>
-    <col min="6" max="6" width="2.23046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.07421875" customWidth="1"/>
-    <col min="10" max="10" width="9.23046875" style="8"/>
-    <col min="11" max="11" width="2.23046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.3046875" customWidth="1"/>
-    <col min="15" max="15" width="9.23046875" style="8"/>
-    <col min="20" max="20" width="9.23046875" style="8"/>
-    <col min="25" max="25" width="9.23046875" style="8"/>
+    <col min="1" max="1" width="2.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="13"/>
+    <col min="4" max="4" width="12.85546875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="7"/>
+    <col min="6" max="6" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="8"/>
+    <col min="11" max="11" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="8"/>
+    <col min="20" max="20" width="9.28515625" style="8"/>
+    <col min="25" max="25" width="9.28515625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -4304,7 +4303,7 @@
       <c r="T1" s="22"/>
       <c r="Y1" s="22"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
@@ -4332,7 +4331,7 @@
       <c r="X2" s="11"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -4352,7 +4351,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>31</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -4410,129 +4409,86 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="Y8" s="8"/>
+    </row>
+    <row r="9" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="7"/>
+      <c r="J9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="Y9" s="8"/>
+    </row>
+    <row r="10" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="7"/>
+      <c r="J10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="Y10" s="8"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A9" s="14"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A10" s="14"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A11" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" t="s">
-        <v>114</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="E14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>54</v>
       </c>
       <c r="I14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="D15" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>8</v>
@@ -4542,21 +4498,21 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>172</v>
+        <v>76</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>8</v>
@@ -4568,139 +4524,136 @@
         <v>76</v>
       </c>
       <c r="I16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" t="s">
         <v>117</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A18" s="14"/>
-      <c r="B18" s="3" t="s">
+      <c r="J19" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="G18" s="17" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A20" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="O20" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A21" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A22" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>105</v>
-      </c>
       <c r="E22" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="13" t="s">
         <v>54</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="O22" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="D23" s="13" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>8</v>
@@ -4711,21 +4664,21 @@
       <c r="L23" s="9"/>
       <c r="M23" s="13"/>
       <c r="N23" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O23" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>172</v>
+        <v>76</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>8</v>
@@ -4738,439 +4691,207 @@
         <v>76</v>
       </c>
       <c r="N24" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="9"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" s="9"/>
+      <c r="M27" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N27" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="O24" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="B25" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="13" t="s">
+      <c r="O27" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="L29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="18"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L26" s="17" t="s">
+      <c r="D32" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="18"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A27" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A28" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A29" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A30" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A31" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A35" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A37" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A38" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A39" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A40" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A42" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A43" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A44" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A45" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A46" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A47" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A48" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A49" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A50" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A52" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A53" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A54" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A55" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A56" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A57" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B65" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="18"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5179,22 +4900,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77354914-ED13-49AE-B0F1-7F945F881C48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.15234375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.23046875" style="13" customWidth="1"/>
-    <col min="3" max="4" width="9.23046875" style="13"/>
-    <col min="5" max="5" width="11.921875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="13" customWidth="1"/>
+    <col min="3" max="4" width="9.28515625" style="13"/>
+    <col min="5" max="5" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -5205,7 +4926,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>27</v>
       </c>
@@ -5213,7 +4934,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -5221,7 +4942,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>31</v>
       </c>
@@ -5232,7 +4953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -5243,26 +4964,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>43</v>
@@ -5271,12 +4992,12 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>56</v>
@@ -5285,7 +5006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
@@ -5299,12 +5020,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>63</v>
@@ -5313,16 +5034,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="3" t="s">
         <v>44</v>
@@ -5331,12 +5052,12 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>55</v>
@@ -5345,7 +5066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
@@ -5359,12 +5080,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>62</v>
@@ -5373,7 +5094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>31</v>
       </c>
@@ -5381,13 +5102,13 @@
         <v>47</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>29</v>
       </c>
@@ -5395,13 +5116,13 @@
         <v>47</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>31</v>
       </c>
@@ -5409,13 +5130,13 @@
         <v>47</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>29</v>
       </c>
@@ -5423,13 +5144,13 @@
         <v>47</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
         <v>52</v>
       </c>
@@ -5443,23 +5164,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA65B74B-5DA1-4137-A045-0809C3DDDFED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.765625" customWidth="1"/>
-    <col min="2" max="2" width="4.61328125" customWidth="1"/>
-    <col min="3" max="3" width="6.61328125" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.07421875" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -5479,7 +5200,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
@@ -5495,7 +5216,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -5507,7 +5228,7 @@
       <c r="I3" s="13"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>28</v>
@@ -5523,7 +5244,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>168</v>
       </c>
@@ -5547,7 +5268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
@@ -5571,7 +5292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -5583,10 +5304,10 @@
       <c r="I7" s="13"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5603,14 +5324,14 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>8</v>
@@ -5627,7 +5348,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -5645,7 +5366,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
@@ -5671,7 +5392,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
@@ -5697,7 +5418,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>31</v>
       </c>
@@ -5721,7 +5442,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -5739,7 +5460,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
@@ -5765,7 +5486,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>31</v>
       </c>
@@ -5785,7 +5506,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
@@ -5803,7 +5524,7 @@
       <c r="I17" s="13"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -5815,7 +5536,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="17" t="s">
         <v>52</v>
@@ -5829,7 +5550,7 @@
       <c r="I19" s="13"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -5837,13 +5558,13 @@
       <c r="E20" s="7"/>
       <c r="F20" s="13"/>
       <c r="G20" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -5855,7 +5576,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -5875,7 +5596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -5895,7 +5616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5915,7 +5636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -5935,7 +5656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -5955,7 +5676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -5975,7 +5696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -5995,7 +5716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -6007,7 +5728,7 @@
       <c r="I29" s="13"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -6027,7 +5748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -6047,7 +5768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -6067,7 +5788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -6087,7 +5808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -6107,7 +5828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -6127,7 +5848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -6147,7 +5868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -6159,7 +5880,7 @@
       <c r="I37" s="13"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -6179,7 +5900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -6199,7 +5920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -6219,7 +5940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -6239,7 +5960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -6259,7 +5980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -6279,7 +6000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -6299,7 +6020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -6319,7 +6040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -6339,7 +6060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -6351,7 +6072,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -6371,7 +6092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -6391,7 +6112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -6411,7 +6132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -6431,7 +6152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -6451,7 +6172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -6471,7 +6192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -6483,7 +6204,7 @@
       <c r="I54" s="13"/>
       <c r="J54" s="7"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -6495,7 +6216,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -6509,28 +6230,28 @@
       <c r="I56" s="17"/>
       <c r="J56" s="18"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>

</xml_diff>